<commit_message>
reduced the memory and some small changes
</commit_message>
<xml_diff>
--- a/learningAgents/src/optim_PGM_base/results.xlsx
+++ b/learningAgents/src/optim_PGM_base/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjaha\Documents\EquiLearn\optim_PGM_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD42919D-ADD3-4215-9477-E4179C86596A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0DFBC-B97D-4F34-88BE-48B43EFEE67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,11 +406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,6 +528,156 @@
       <c r="D11"/>
       <c r="E11"/>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>